<commit_message>
Updated documentation and PowerPoint.
</commit_message>
<xml_diff>
--- a/Planning and Design/CST-247-RS-SprintProductLog - CLC.xlsx
+++ b/Planning and Design/CST-247-RS-SprintProductLog - CLC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Grand Canyon University\Classes\CST-247\CLC - Week 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Grand Canyon University\Classes\CST-247\CLC - Week 7\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>User Stories</t>
   </si>
@@ -147,6 +147,30 @@
   </si>
   <si>
     <t>Project Title: Minesweeper Web Application</t>
+  </si>
+  <si>
+    <t>Nlog log reporting</t>
+  </si>
+  <si>
+    <t>Application Management</t>
+  </si>
+  <si>
+    <t>Track what the user is doing and any errors</t>
+  </si>
+  <si>
+    <t>AJAX Partial View</t>
+  </si>
+  <si>
+    <t>Avoid page refreshes</t>
+  </si>
+  <si>
+    <t>Refactor the game board to utilize AJAX partials views as the display.</t>
+  </si>
+  <si>
+    <t>Users will avoid seeing page refreshrs during game play.</t>
+  </si>
+  <si>
+    <t>The application can offer the best functionality.</t>
   </si>
 </sst>
 </file>
@@ -314,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -352,8 +376,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,9 +404,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,15 +686,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2060"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="82.140625" bestFit="1" customWidth="1"/>
@@ -671,14 +704,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -687,11 +720,11 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="5"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -747,10 +780,10 @@
       <c r="G4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="17">
         <v>44065</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -777,7 +810,7 @@
       <c r="H5" s="16">
         <v>44058</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -804,7 +837,9 @@
       <c r="H6" s="16">
         <v>44058</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="19">
+        <v>44079</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -831,7 +866,9 @@
       <c r="H7" s="16">
         <v>44058</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="19">
+        <v>44079</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -855,8 +892,12 @@
       <c r="G8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="16">
+        <v>44079</v>
+      </c>
+      <c r="I8" s="19">
+        <v>44086</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -880,55 +921,91 @@
       <c r="G9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="16">
+        <v>44087</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>38</v>
+      <c r="E10" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="7"/>
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="16">
+        <v>44087</v>
+      </c>
+      <c r="I11" s="19">
+        <v>44091</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="7"/>
+      <c r="A12" s="8">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="17">
+        <v>44087</v>
+      </c>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
@@ -938,8 +1015,8 @@
       <c r="E13" s="6"/>
       <c r="F13" s="13"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
@@ -949,8 +1026,8 @@
       <c r="E14" s="6"/>
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -960,8 +1037,8 @@
       <c r="E15" s="6"/>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -971,8 +1048,8 @@
       <c r="E16" s="6"/>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
@@ -982,8 +1059,8 @@
       <c r="E17" s="6"/>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="7"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
@@ -993,8 +1070,8 @@
       <c r="E18" s="6"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -1004,8 +1081,8 @@
       <c r="E19" s="6"/>
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
@@ -1015,8 +1092,8 @@
       <c r="E20" s="6"/>
       <c r="F20" s="13"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -1026,8 +1103,8 @@
       <c r="E21" s="6"/>
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="7"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
@@ -1037,8 +1114,8 @@
       <c r="E22" s="6"/>
       <c r="F22" s="13"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="7"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
@@ -1048,8 +1125,8 @@
       <c r="E23" s="6"/>
       <c r="F23" s="13"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="7"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
@@ -1059,8 +1136,8 @@
       <c r="E24" s="6"/>
       <c r="F24" s="13"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="7"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
@@ -1070,8 +1147,8 @@
       <c r="E25" s="6"/>
       <c r="F25" s="13"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="7"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
@@ -1081,8 +1158,8 @@
       <c r="E26" s="6"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="7"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
@@ -1092,8 +1169,8 @@
       <c r="E27" s="6"/>
       <c r="F27" s="13"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="7"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -1103,8 +1180,8 @@
       <c r="E28" s="6"/>
       <c r="F28" s="13"/>
       <c r="G28" s="14"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="7"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
@@ -1114,8 +1191,8 @@
       <c r="E29" s="6"/>
       <c r="F29" s="13"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="7"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
@@ -1125,8 +1202,8 @@
       <c r="E30" s="6"/>
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="7"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
@@ -1136,8 +1213,8 @@
       <c r="E31" s="6"/>
       <c r="F31" s="13"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="7"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
@@ -1147,8 +1224,8 @@
       <c r="E32" s="6"/>
       <c r="F32" s="13"/>
       <c r="G32" s="14"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="7"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
@@ -1158,8 +1235,8 @@
       <c r="E33" s="6"/>
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="7"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
@@ -1169,8 +1246,8 @@
       <c r="E34" s="6"/>
       <c r="F34" s="13"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="7"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
@@ -1180,8 +1257,8 @@
       <c r="E35" s="6"/>
       <c r="F35" s="13"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="7"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
@@ -1191,8 +1268,8 @@
       <c r="E36" s="6"/>
       <c r="F36" s="13"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="7"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
@@ -1202,8 +1279,8 @@
       <c r="E37" s="6"/>
       <c r="F37" s="13"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="7"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
@@ -1213,8 +1290,8 @@
       <c r="E38" s="6"/>
       <c r="F38" s="13"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="7"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
@@ -1224,8 +1301,8 @@
       <c r="E39" s="6"/>
       <c r="F39" s="13"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="7"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
@@ -1235,7 +1312,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="13"/>
       <c r="G40" s="14"/>
-      <c r="H40" s="11"/>
+      <c r="H40" s="20"/>
       <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1246,7 +1323,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="13"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="11"/>
+      <c r="H41" s="20"/>
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1257,7 +1334,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="13"/>
       <c r="G42" s="14"/>
-      <c r="H42" s="11"/>
+      <c r="H42" s="20"/>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1268,7 +1345,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="13"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="11"/>
+      <c r="H43" s="20"/>
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1279,7 +1356,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="13"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="11"/>
+      <c r="H44" s="20"/>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -23468,15 +23545,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1251" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c2c36359d71eb747fbb188f75fc8d29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08acee74153637279a480e75df712a71" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23665,7 +23733,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -23674,15 +23742,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347394F-0C4E-4E34-9270-1B2FF1850191}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23701,7 +23770,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -23709,4 +23778,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>